<commit_message>
Added my notebook for the xgboost model after hyperparameter tuning
</commit_message>
<xml_diff>
--- a/Code/shane/data_dictionary_template.xlsx
+++ b/Code/shane/data_dictionary_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03ee8b6fdc2ba255/Documents/School/08. Spring 2024/Mortgage-Analysis-Project/Code/shane/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_458541F7809B892E8F2D4C8CBD6935557878EAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16EB1FD3-491F-47E4-BFC3-DCA439F6636A}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="11_458541F7809B892E8F2D4C8CBD6935557878EAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33865846-E57B-4D51-B505-5CB7EE3019D2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29310" yWindow="-8145" windowWidth="15450" windowHeight="23805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1485,6 +1485,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1776,13 +1780,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="70.5703125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>